<commit_message>
Excel-Datei aktualisiert mit den neuesten Daten
</commit_message>
<xml_diff>
--- a/license.xlsx
+++ b/license.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8863138e69c67576/Projekte/Datahunter/License/datahunter_license/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CA3512-D027-408D-8F1F-D885DEFAD5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{80CA3512-D027-408D-8F1F-D885DEFAD5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7878BC2E-0FB5-4A30-AD03-5D2D267066AE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{E73852FC-569D-4DD7-B537-3E3D9B6C59F5}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>56290</v>
+        <v>59942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>